<commit_message>
added a text file and edited it
</commit_message>
<xml_diff>
--- a/NewVersion2.xlsx
+++ b/NewVersion2.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>how to</t>
+  </si>
+  <si>
+    <t>fadfdsfas</t>
   </si>
 </sst>
 </file>
@@ -358,17 +361,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G7"/>
+  <dimension ref="G7:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>